<commit_message>
modified:   DataLoader.py 	modified:   Exports/TeamExport_A46051_Alpha_M_Period 3.xlsx 	modified:   Scraper.py 	modified:   __pycache__/Brands.cpython-311.pyc 	modified:   __pycache__/DataLoader.cpython-311.pyc 	modified:   __pycache__/Scraper.cpython-311.pyc 	new file:   attributes.json 	modified:   main.ipynb 	modified:   test_scraper.ipynb
</commit_message>
<xml_diff>
--- a/Exports/TeamExport_A46051_Alpha_M_Period 3.xlsx
+++ b/Exports/TeamExport_A46051_Alpha_M_Period 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Anno III\UCSD\112\Markstrat\Code\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC9222-1960-42C7-A134-FB693E61CF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66332B2F-71BC-4A10-B2F3-8B4B2BDCCB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Firm" sheetId="1" r:id="rId1"/>
@@ -2408,6 +2408,9 @@
     <xf numFmtId="4" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2443,9 +2446,6 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3958,25 +3958,25 @@
     </row>
     <row r="66" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B66" s="82"/>
-      <c r="D66" s="319"/>
-      <c r="E66" s="320"/>
-      <c r="F66" s="323" t="s">
+      <c r="D66" s="320"/>
+      <c r="E66" s="321"/>
+      <c r="F66" s="324" t="s">
         <v>39</v>
       </c>
-      <c r="G66" s="324"/>
-      <c r="H66" s="324"/>
-      <c r="I66" s="325"/>
-      <c r="J66" s="323" t="s">
+      <c r="G66" s="325"/>
+      <c r="H66" s="325"/>
+      <c r="I66" s="326"/>
+      <c r="J66" s="324" t="s">
         <v>40</v>
       </c>
-      <c r="K66" s="324"/>
-      <c r="L66" s="324"/>
-      <c r="M66" s="325"/>
+      <c r="K66" s="325"/>
+      <c r="L66" s="325"/>
+      <c r="M66" s="326"/>
     </row>
     <row r="67" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B67" s="82"/>
-      <c r="D67" s="321"/>
-      <c r="E67" s="322"/>
+      <c r="D67" s="322"/>
+      <c r="E67" s="323"/>
       <c r="F67" s="83" t="s">
         <v>41</v>
       </c>
@@ -5557,8 +5557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7754,7 +7754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O592"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A369" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A369" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E383" sqref="E383"/>
     </sheetView>
   </sheetViews>
@@ -7813,10 +7813,10 @@
     </row>
     <row r="5" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="82"/>
-      <c r="D5" s="321" t="s">
+      <c r="D5" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="322"/>
+      <c r="E5" s="323"/>
       <c r="F5" s="178" t="s">
         <v>125</v>
       </c>
@@ -8334,10 +8334,10 @@
     </row>
     <row r="38" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="82"/>
-      <c r="D38" s="321" t="s">
+      <c r="D38" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="322"/>
+      <c r="E38" s="323"/>
       <c r="F38" s="178" t="s">
         <v>125</v>
       </c>
@@ -8883,10 +8883,10 @@
     </row>
     <row r="72" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="82"/>
-      <c r="D72" s="321" t="s">
+      <c r="D72" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E72" s="322"/>
+      <c r="E72" s="323"/>
       <c r="F72" s="152" t="s">
         <v>126</v>
       </c>
@@ -9035,10 +9035,10 @@
     </row>
     <row r="82" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B82" s="82"/>
-      <c r="D82" s="321" t="s">
+      <c r="D82" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E82" s="322"/>
+      <c r="E82" s="323"/>
       <c r="F82" s="178" t="s">
         <v>132</v>
       </c>
@@ -9585,10 +9585,10 @@
     </row>
     <row r="116" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B116" s="82"/>
-      <c r="D116" s="321" t="s">
+      <c r="D116" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E116" s="322"/>
+      <c r="E116" s="323"/>
       <c r="F116" s="178" t="s">
         <v>132</v>
       </c>
@@ -10178,27 +10178,27 @@
     </row>
     <row r="152" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B152" s="82"/>
-      <c r="D152" s="319" t="s">
+      <c r="D152" s="320" t="s">
         <v>56</v>
       </c>
-      <c r="E152" s="320"/>
-      <c r="F152" s="323" t="s">
+      <c r="E152" s="321"/>
+      <c r="F152" s="324" t="s">
         <v>36</v>
       </c>
-      <c r="G152" s="324"/>
-      <c r="H152" s="324"/>
-      <c r="I152" s="325"/>
-      <c r="J152" s="323" t="s">
+      <c r="G152" s="325"/>
+      <c r="H152" s="325"/>
+      <c r="I152" s="326"/>
+      <c r="J152" s="324" t="s">
         <v>40</v>
       </c>
-      <c r="K152" s="324"/>
-      <c r="L152" s="324"/>
-      <c r="M152" s="325"/>
+      <c r="K152" s="325"/>
+      <c r="L152" s="325"/>
+      <c r="M152" s="326"/>
     </row>
     <row r="153" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B153" s="82"/>
-      <c r="D153" s="321"/>
-      <c r="E153" s="322"/>
+      <c r="D153" s="322"/>
+      <c r="E153" s="323"/>
       <c r="F153" s="83" t="s">
         <v>41</v>
       </c>
@@ -10823,27 +10823,27 @@
     </row>
     <row r="187" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B187" s="82"/>
-      <c r="D187" s="319" t="s">
+      <c r="D187" s="320" t="s">
         <v>56</v>
       </c>
-      <c r="E187" s="320"/>
-      <c r="F187" s="323" t="s">
+      <c r="E187" s="321"/>
+      <c r="F187" s="324" t="s">
         <v>39</v>
       </c>
-      <c r="G187" s="324"/>
-      <c r="H187" s="324"/>
-      <c r="I187" s="325"/>
-      <c r="J187" s="323" t="s">
+      <c r="G187" s="325"/>
+      <c r="H187" s="325"/>
+      <c r="I187" s="326"/>
+      <c r="J187" s="324" t="s">
         <v>140</v>
       </c>
-      <c r="K187" s="324"/>
-      <c r="L187" s="324"/>
-      <c r="M187" s="325"/>
+      <c r="K187" s="325"/>
+      <c r="L187" s="325"/>
+      <c r="M187" s="326"/>
     </row>
     <row r="188" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B188" s="82"/>
-      <c r="D188" s="321"/>
-      <c r="E188" s="322"/>
+      <c r="D188" s="322"/>
+      <c r="E188" s="323"/>
       <c r="F188" s="83" t="s">
         <v>41</v>
       </c>
@@ -11450,7 +11450,7 @@
     </row>
     <row r="223" spans="1:13" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="82"/>
-      <c r="E223" s="331" t="s">
+      <c r="E223" s="319" t="s">
         <v>56</v>
       </c>
       <c r="F223" s="152" t="s">
@@ -12702,7 +12702,7 @@
     </row>
     <row r="296" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B296" s="82"/>
-      <c r="E296" s="331" t="s">
+      <c r="E296" s="319" t="s">
         <v>56</v>
       </c>
       <c r="F296" s="152" t="s">
@@ -13650,10 +13650,10 @@
     </row>
     <row r="362" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B362" s="82"/>
-      <c r="D362" s="321" t="s">
+      <c r="D362" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E362" s="322"/>
+      <c r="E362" s="323"/>
       <c r="F362" s="152" t="s">
         <v>151</v>
       </c>
@@ -13790,10 +13790,10 @@
     </row>
     <row r="372" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B372" s="82"/>
-      <c r="D372" s="321" t="s">
+      <c r="D372" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E372" s="322"/>
+      <c r="E372" s="323"/>
       <c r="F372" s="178" t="s">
         <v>132</v>
       </c>
@@ -13985,7 +13985,7 @@
     </row>
     <row r="383" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B383" s="82"/>
-      <c r="E383" s="331" t="s">
+      <c r="E383" s="319" t="s">
         <v>56</v>
       </c>
       <c r="F383" s="178" t="s">
@@ -14514,10 +14514,10 @@
     </row>
     <row r="418" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B418" s="82"/>
-      <c r="D418" s="321" t="s">
+      <c r="D418" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E418" s="322"/>
+      <c r="E418" s="323"/>
       <c r="F418" s="138" t="s">
         <v>165</v>
       </c>
@@ -14971,10 +14971,10 @@
     </row>
     <row r="454" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B454" s="82"/>
-      <c r="D454" s="321" t="s">
+      <c r="D454" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E454" s="322"/>
+      <c r="E454" s="323"/>
       <c r="F454" s="178" t="s">
         <v>132</v>
       </c>
@@ -15135,10 +15135,10 @@
     </row>
     <row r="464" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B464" s="82"/>
-      <c r="D464" s="321" t="s">
+      <c r="D464" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E464" s="322"/>
+      <c r="E464" s="323"/>
       <c r="F464" s="178" t="s">
         <v>132</v>
       </c>
@@ -15647,10 +15647,10 @@
     </row>
     <row r="499" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B499" s="82"/>
-      <c r="D499" s="321" t="s">
+      <c r="D499" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E499" s="322"/>
+      <c r="E499" s="323"/>
       <c r="F499" s="152" t="s">
         <v>126</v>
       </c>
@@ -15762,10 +15762,10 @@
     </row>
     <row r="507" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B507" s="82"/>
-      <c r="D507" s="321" t="s">
+      <c r="D507" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E507" s="322"/>
+      <c r="E507" s="323"/>
       <c r="F507" s="277" t="s">
         <v>126</v>
       </c>
@@ -15871,10 +15871,10 @@
     </row>
     <row r="515" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B515" s="82"/>
-      <c r="D515" s="321" t="s">
+      <c r="D515" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E515" s="321"/>
+      <c r="E515" s="322"/>
       <c r="F515" s="281"/>
     </row>
     <row r="516" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -15963,10 +15963,10 @@
     </row>
     <row r="525" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B525" s="82"/>
-      <c r="D525" s="321" t="s">
+      <c r="D525" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E525" s="322"/>
+      <c r="E525" s="323"/>
       <c r="F525" s="152" t="s">
         <v>41</v>
       </c>
@@ -16063,10 +16063,10 @@
     </row>
     <row r="533" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B533" s="82"/>
-      <c r="D533" s="321" t="s">
+      <c r="D533" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E533" s="322"/>
+      <c r="E533" s="323"/>
       <c r="F533" s="152" t="s">
         <v>41</v>
       </c>
@@ -16155,10 +16155,10 @@
     </row>
     <row r="541" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B541" s="82"/>
-      <c r="D541" s="321" t="s">
+      <c r="D541" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E541" s="321"/>
+      <c r="E541" s="322"/>
       <c r="F541" s="281"/>
     </row>
     <row r="542" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -16248,28 +16248,28 @@
     </row>
     <row r="551" spans="1:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B551" s="9"/>
-      <c r="F551" s="328" t="s">
+      <c r="F551" s="329" t="s">
         <v>184</v>
       </c>
-      <c r="G551" s="329"/>
-      <c r="H551" s="330"/>
-      <c r="I551" s="328" t="s">
+      <c r="G551" s="330"/>
+      <c r="H551" s="331"/>
+      <c r="I551" s="329" t="s">
         <v>185</v>
       </c>
-      <c r="J551" s="329"/>
-      <c r="K551" s="330"/>
-      <c r="L551" s="328" t="s">
+      <c r="J551" s="330"/>
+      <c r="K551" s="331"/>
+      <c r="L551" s="329" t="s">
         <v>186</v>
       </c>
-      <c r="M551" s="329"/>
-      <c r="N551" s="330"/>
+      <c r="M551" s="330"/>
+      <c r="N551" s="331"/>
     </row>
     <row r="552" spans="1:14" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B552" s="82"/>
-      <c r="D552" s="321" t="s">
+      <c r="D552" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E552" s="321"/>
+      <c r="E552" s="322"/>
       <c r="F552" s="83" t="s">
         <v>5</v>
       </c>
@@ -16552,10 +16552,10 @@
     </row>
     <row r="563" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B563" s="82"/>
-      <c r="D563" s="321" t="s">
+      <c r="D563" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E563" s="322"/>
+      <c r="E563" s="323"/>
       <c r="F563" s="152" t="s">
         <v>126</v>
       </c>
@@ -16696,29 +16696,29 @@
     <row r="571" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A571" s="3"/>
       <c r="B571" s="9"/>
-      <c r="F571" s="326" t="s">
+      <c r="F571" s="327" t="s">
         <v>194</v>
       </c>
-      <c r="G571" s="327"/>
-      <c r="H571" s="326" t="s">
+      <c r="G571" s="328"/>
+      <c r="H571" s="327" t="s">
         <v>196</v>
       </c>
-      <c r="I571" s="327"/>
-      <c r="J571" s="326" t="s">
+      <c r="I571" s="328"/>
+      <c r="J571" s="327" t="s">
         <v>110</v>
       </c>
-      <c r="K571" s="327"/>
-      <c r="L571" s="326" t="s">
+      <c r="K571" s="328"/>
+      <c r="L571" s="327" t="s">
         <v>143</v>
       </c>
-      <c r="M571" s="327"/>
+      <c r="M571" s="328"/>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A572" s="3"/>
-      <c r="D572" s="321" t="s">
+      <c r="D572" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="E572" s="322"/>
+      <c r="E572" s="323"/>
       <c r="F572" s="297" t="s">
         <v>197</v>
       </c>
@@ -17344,6 +17344,24 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D572:E572"/>
+    <mergeCell ref="F187:I187"/>
+    <mergeCell ref="J187:M187"/>
+    <mergeCell ref="D152:E153"/>
+    <mergeCell ref="F152:I152"/>
+    <mergeCell ref="J152:M152"/>
+    <mergeCell ref="D362:E362"/>
+    <mergeCell ref="D372:E372"/>
+    <mergeCell ref="D187:E188"/>
+    <mergeCell ref="D552:E552"/>
+    <mergeCell ref="D454:E454"/>
+    <mergeCell ref="D464:E464"/>
+    <mergeCell ref="D499:E499"/>
     <mergeCell ref="D418:E418"/>
     <mergeCell ref="L571:M571"/>
     <mergeCell ref="F571:G571"/>
@@ -17358,24 +17376,6 @@
     <mergeCell ref="D525:E525"/>
     <mergeCell ref="D533:E533"/>
     <mergeCell ref="D541:E541"/>
-    <mergeCell ref="D572:E572"/>
-    <mergeCell ref="F187:I187"/>
-    <mergeCell ref="J187:M187"/>
-    <mergeCell ref="D152:E153"/>
-    <mergeCell ref="F152:I152"/>
-    <mergeCell ref="J152:M152"/>
-    <mergeCell ref="D362:E362"/>
-    <mergeCell ref="D372:E372"/>
-    <mergeCell ref="D187:E188"/>
-    <mergeCell ref="D552:E552"/>
-    <mergeCell ref="D454:E454"/>
-    <mergeCell ref="D464:E464"/>
-    <mergeCell ref="D499:E499"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D116:E116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17445,10 +17445,10 @@
     </row>
     <row r="5" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="82"/>
-      <c r="D5" s="321" t="s">
+      <c r="D5" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="322"/>
+      <c r="E5" s="323"/>
       <c r="F5" s="178" t="s">
         <v>125</v>
       </c>
@@ -17804,10 +17804,10 @@
     </row>
     <row r="38" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="82"/>
-      <c r="D38" s="321" t="s">
+      <c r="D38" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="322"/>
+      <c r="E38" s="323"/>
       <c r="F38" s="178" t="s">
         <v>125</v>
       </c>
@@ -18191,10 +18191,10 @@
     </row>
     <row r="72" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="82"/>
-      <c r="D72" s="321" t="s">
+      <c r="D72" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E72" s="322"/>
+      <c r="E72" s="323"/>
       <c r="F72" s="152" t="s">
         <v>201</v>
       </c>
@@ -18305,10 +18305,10 @@
     </row>
     <row r="82" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B82" s="82"/>
-      <c r="D82" s="321" t="s">
+      <c r="D82" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E82" s="322"/>
+      <c r="E82" s="323"/>
       <c r="F82" s="178" t="s">
         <v>132</v>
       </c>
@@ -18693,10 +18693,10 @@
     </row>
     <row r="116" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B116" s="82"/>
-      <c r="D116" s="321" t="s">
+      <c r="D116" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E116" s="322"/>
+      <c r="E116" s="323"/>
       <c r="F116" s="178" t="s">
         <v>132</v>
       </c>
@@ -19124,27 +19124,27 @@
     </row>
     <row r="152" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B152" s="82"/>
-      <c r="D152" s="319" t="s">
+      <c r="D152" s="320" t="s">
         <v>74</v>
       </c>
-      <c r="E152" s="320"/>
-      <c r="F152" s="323" t="s">
+      <c r="E152" s="321"/>
+      <c r="F152" s="324" t="s">
         <v>36</v>
       </c>
-      <c r="G152" s="324"/>
-      <c r="H152" s="324"/>
-      <c r="I152" s="325"/>
-      <c r="J152" s="323" t="s">
+      <c r="G152" s="325"/>
+      <c r="H152" s="325"/>
+      <c r="I152" s="326"/>
+      <c r="J152" s="324" t="s">
         <v>40</v>
       </c>
-      <c r="K152" s="324"/>
-      <c r="L152" s="324"/>
-      <c r="M152" s="325"/>
+      <c r="K152" s="325"/>
+      <c r="L152" s="325"/>
+      <c r="M152" s="326"/>
     </row>
     <row r="153" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B153" s="82"/>
-      <c r="D153" s="321"/>
-      <c r="E153" s="322"/>
+      <c r="D153" s="322"/>
+      <c r="E153" s="323"/>
       <c r="F153" s="83" t="s">
         <v>41</v>
       </c>
@@ -19613,27 +19613,27 @@
     </row>
     <row r="187" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B187" s="82"/>
-      <c r="D187" s="319" t="s">
+      <c r="D187" s="320" t="s">
         <v>74</v>
       </c>
-      <c r="E187" s="320"/>
-      <c r="F187" s="323" t="s">
+      <c r="E187" s="321"/>
+      <c r="F187" s="324" t="s">
         <v>39</v>
       </c>
-      <c r="G187" s="324"/>
-      <c r="H187" s="324"/>
-      <c r="I187" s="325"/>
-      <c r="J187" s="323" t="s">
+      <c r="G187" s="325"/>
+      <c r="H187" s="325"/>
+      <c r="I187" s="326"/>
+      <c r="J187" s="324" t="s">
         <v>140</v>
       </c>
-      <c r="K187" s="324"/>
-      <c r="L187" s="324"/>
-      <c r="M187" s="325"/>
+      <c r="K187" s="325"/>
+      <c r="L187" s="325"/>
+      <c r="M187" s="326"/>
     </row>
     <row r="188" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B188" s="82"/>
-      <c r="D188" s="321"/>
-      <c r="E188" s="322"/>
+      <c r="D188" s="322"/>
+      <c r="E188" s="323"/>
       <c r="F188" s="83" t="s">
         <v>41</v>
       </c>
@@ -20084,10 +20084,10 @@
     </row>
     <row r="223" spans="1:13" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="82"/>
-      <c r="D223" s="321" t="s">
+      <c r="D223" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E223" s="322"/>
+      <c r="E223" s="323"/>
       <c r="F223" s="152" t="s">
         <v>75</v>
       </c>
@@ -21081,10 +21081,10 @@
     </row>
     <row r="296" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B296" s="82"/>
-      <c r="D296" s="321" t="s">
+      <c r="D296" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E296" s="322"/>
+      <c r="E296" s="323"/>
       <c r="F296" s="152" t="s">
         <v>209</v>
       </c>
@@ -21764,10 +21764,10 @@
     </row>
     <row r="362" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B362" s="82"/>
-      <c r="D362" s="321" t="s">
+      <c r="D362" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E362" s="322"/>
+      <c r="E362" s="323"/>
       <c r="F362" s="152" t="s">
         <v>209</v>
       </c>
@@ -21858,10 +21858,10 @@
     </row>
     <row r="372" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B372" s="82"/>
-      <c r="D372" s="321" t="s">
+      <c r="D372" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E372" s="322"/>
+      <c r="E372" s="323"/>
       <c r="F372" s="178" t="s">
         <v>132</v>
       </c>
@@ -21995,10 +21995,10 @@
     </row>
     <row r="383" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B383" s="82"/>
-      <c r="D383" s="321" t="s">
+      <c r="D383" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E383" s="322"/>
+      <c r="E383" s="323"/>
       <c r="F383" s="178" t="s">
         <v>132</v>
       </c>
@@ -22393,10 +22393,10 @@
     </row>
     <row r="418" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B418" s="82"/>
-      <c r="D418" s="321" t="s">
+      <c r="D418" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E418" s="322"/>
+      <c r="E418" s="323"/>
       <c r="F418" s="138" t="s">
         <v>165</v>
       </c>
@@ -22772,10 +22772,10 @@
     </row>
     <row r="454" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B454" s="82"/>
-      <c r="D454" s="321" t="s">
+      <c r="D454" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E454" s="322"/>
+      <c r="E454" s="323"/>
       <c r="F454" s="178" t="s">
         <v>132</v>
       </c>
@@ -22898,10 +22898,10 @@
     </row>
     <row r="464" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B464" s="82"/>
-      <c r="D464" s="321" t="s">
+      <c r="D464" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E464" s="322"/>
+      <c r="E464" s="323"/>
       <c r="F464" s="178" t="s">
         <v>132</v>
       </c>
@@ -23292,10 +23292,10 @@
     </row>
     <row r="499" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B499" s="82"/>
-      <c r="D499" s="321" t="s">
+      <c r="D499" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E499" s="322"/>
+      <c r="E499" s="323"/>
       <c r="F499" s="152" t="s">
         <v>201</v>
       </c>
@@ -23377,10 +23377,10 @@
     </row>
     <row r="507" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B507" s="82"/>
-      <c r="D507" s="321" t="s">
+      <c r="D507" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E507" s="322"/>
+      <c r="E507" s="323"/>
       <c r="F507" s="277" t="s">
         <v>201</v>
       </c>
@@ -23456,10 +23456,10 @@
     </row>
     <row r="515" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B515" s="82"/>
-      <c r="D515" s="321" t="s">
+      <c r="D515" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E515" s="321"/>
+      <c r="E515" s="322"/>
       <c r="F515" s="281"/>
     </row>
     <row r="516" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -23538,10 +23538,10 @@
     </row>
     <row r="525" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B525" s="82"/>
-      <c r="D525" s="321" t="s">
+      <c r="D525" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E525" s="322"/>
+      <c r="E525" s="323"/>
       <c r="F525" s="152" t="s">
         <v>41</v>
       </c>
@@ -23620,10 +23620,10 @@
     </row>
     <row r="533" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B533" s="82"/>
-      <c r="D533" s="321" t="s">
+      <c r="D533" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E533" s="322"/>
+      <c r="E533" s="323"/>
       <c r="F533" s="152" t="s">
         <v>41</v>
       </c>
@@ -23694,10 +23694,10 @@
     </row>
     <row r="541" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B541" s="82"/>
-      <c r="D541" s="321" t="s">
+      <c r="D541" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E541" s="321"/>
+      <c r="E541" s="322"/>
       <c r="F541" s="281"/>
     </row>
     <row r="542" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -23777,28 +23777,28 @@
     </row>
     <row r="551" spans="1:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B551" s="9"/>
-      <c r="F551" s="328" t="s">
+      <c r="F551" s="329" t="s">
         <v>184</v>
       </c>
-      <c r="G551" s="329"/>
-      <c r="H551" s="330"/>
-      <c r="I551" s="328" t="s">
+      <c r="G551" s="330"/>
+      <c r="H551" s="331"/>
+      <c r="I551" s="329" t="s">
         <v>185</v>
       </c>
-      <c r="J551" s="329"/>
-      <c r="K551" s="330"/>
-      <c r="L551" s="328" t="s">
+      <c r="J551" s="330"/>
+      <c r="K551" s="331"/>
+      <c r="L551" s="329" t="s">
         <v>186</v>
       </c>
-      <c r="M551" s="329"/>
-      <c r="N551" s="330"/>
+      <c r="M551" s="330"/>
+      <c r="N551" s="331"/>
     </row>
     <row r="552" spans="1:14" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B552" s="82"/>
-      <c r="D552" s="321" t="s">
+      <c r="D552" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E552" s="321"/>
+      <c r="E552" s="322"/>
       <c r="F552" s="83" t="s">
         <v>5</v>
       </c>
@@ -24053,10 +24053,10 @@
     </row>
     <row r="563" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B563" s="82"/>
-      <c r="D563" s="321" t="s">
+      <c r="D563" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E563" s="322"/>
+      <c r="E563" s="323"/>
       <c r="F563" s="152" t="s">
         <v>201</v>
       </c>
@@ -24147,23 +24147,23 @@
     <row r="571" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A571" s="3"/>
       <c r="B571" s="9"/>
-      <c r="F571" s="326" t="s">
+      <c r="F571" s="327" t="s">
         <v>217</v>
       </c>
-      <c r="G571" s="327"/>
-      <c r="H571" s="326"/>
-      <c r="I571" s="327"/>
-      <c r="J571" s="326"/>
-      <c r="K571" s="327"/>
-      <c r="L571" s="326"/>
-      <c r="M571" s="327"/>
+      <c r="G571" s="328"/>
+      <c r="H571" s="327"/>
+      <c r="I571" s="328"/>
+      <c r="J571" s="327"/>
+      <c r="K571" s="328"/>
+      <c r="L571" s="327"/>
+      <c r="M571" s="328"/>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A572" s="3"/>
-      <c r="D572" s="321" t="s">
+      <c r="D572" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="E572" s="322"/>
+      <c r="E572" s="323"/>
       <c r="F572" s="297" t="s">
         <v>197</v>
       </c>
@@ -24461,13 +24461,26 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="D362:E362"/>
-    <mergeCell ref="D372:E372"/>
-    <mergeCell ref="D187:E188"/>
-    <mergeCell ref="F187:I187"/>
-    <mergeCell ref="J187:M187"/>
-    <mergeCell ref="D223:E223"/>
-    <mergeCell ref="D296:E296"/>
+    <mergeCell ref="D572:E572"/>
+    <mergeCell ref="L551:N551"/>
+    <mergeCell ref="D552:E552"/>
+    <mergeCell ref="D563:E563"/>
+    <mergeCell ref="F571:G571"/>
+    <mergeCell ref="H571:I571"/>
+    <mergeCell ref="J571:K571"/>
+    <mergeCell ref="L571:M571"/>
+    <mergeCell ref="D515:E515"/>
+    <mergeCell ref="D525:E525"/>
+    <mergeCell ref="D533:E533"/>
+    <mergeCell ref="F551:H551"/>
+    <mergeCell ref="I551:K551"/>
+    <mergeCell ref="D541:E541"/>
+    <mergeCell ref="D383:E383"/>
+    <mergeCell ref="D454:E454"/>
+    <mergeCell ref="D464:E464"/>
+    <mergeCell ref="D499:E499"/>
+    <mergeCell ref="D507:E507"/>
+    <mergeCell ref="D418:E418"/>
     <mergeCell ref="D152:E153"/>
     <mergeCell ref="F152:I152"/>
     <mergeCell ref="J152:M152"/>
@@ -24476,26 +24489,13 @@
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="D82:E82"/>
     <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D383:E383"/>
-    <mergeCell ref="D454:E454"/>
-    <mergeCell ref="D464:E464"/>
-    <mergeCell ref="D499:E499"/>
-    <mergeCell ref="D507:E507"/>
-    <mergeCell ref="D418:E418"/>
-    <mergeCell ref="D515:E515"/>
-    <mergeCell ref="D525:E525"/>
-    <mergeCell ref="D533:E533"/>
-    <mergeCell ref="F551:H551"/>
-    <mergeCell ref="I551:K551"/>
-    <mergeCell ref="D541:E541"/>
-    <mergeCell ref="D572:E572"/>
-    <mergeCell ref="L551:N551"/>
-    <mergeCell ref="D552:E552"/>
-    <mergeCell ref="D563:E563"/>
-    <mergeCell ref="F571:G571"/>
-    <mergeCell ref="H571:I571"/>
-    <mergeCell ref="J571:K571"/>
-    <mergeCell ref="L571:M571"/>
+    <mergeCell ref="D362:E362"/>
+    <mergeCell ref="D372:E372"/>
+    <mergeCell ref="D187:E188"/>
+    <mergeCell ref="F187:I187"/>
+    <mergeCell ref="J187:M187"/>
+    <mergeCell ref="D223:E223"/>
+    <mergeCell ref="D296:E296"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new margin function+ minor fixes
</commit_message>
<xml_diff>
--- a/Exports/TeamExport_A46051_Alpha_M_Period 3.xlsx
+++ b/Exports/TeamExport_A46051_Alpha_M_Period 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Anno III\UCSD\112\Markstrat\Code\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66332B2F-71BC-4A10-B2F3-8B4B2BDCCB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB4512D-16E9-481B-AF36-A9EBF5DCF198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11565" yWindow="-21720" windowWidth="51840" windowHeight="21120" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Firm" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,38 @@
     <sheet name="Vodites" sheetId="5" r:id="rId4"/>
     <sheet name="INDUSTRY BENCHMARKING" sheetId="7" r:id="rId5"/>
     <sheet name="Studies - Sonites Market" sheetId="8" r:id="rId6"/>
-    <sheet name="Studies - Vodites Market" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId7"/>
+    <sheet name="Studies - Vodites Market" sheetId="9" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">Sheet1!$D$2</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">Sheet1!$D$7</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">103</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterateDelta="9.9999999974897903E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="229">
   <si>
     <t>FINANCIAL REPORT – FIRM M – PERIOD 3</t>
   </si>
@@ -691,16 +721,50 @@
   <si>
     <t>_Conjoint</t>
   </si>
+  <si>
+    <t>rec</t>
+  </si>
+  <si>
+    <t>avg ret</t>
+  </si>
+  <si>
+    <t>av distr m</t>
+  </si>
+  <si>
+    <t>sell p</t>
+  </si>
+  <si>
+    <t>trans</t>
+  </si>
+  <si>
+    <t>MARGIN</t>
+  </si>
+  <si>
+    <t>VECCHIO</t>
+  </si>
+  <si>
+    <t>NUOVO</t>
+  </si>
+  <si>
+    <t>Prod</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -802,6 +866,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1452,7 +1523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="332">
+  <cellXfs count="340">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2411,6 +2482,19 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2446,6 +2530,9 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3958,25 +4045,25 @@
     </row>
     <row r="66" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B66" s="82"/>
-      <c r="D66" s="320"/>
-      <c r="E66" s="321"/>
-      <c r="F66" s="324" t="s">
+      <c r="D66" s="327"/>
+      <c r="E66" s="328"/>
+      <c r="F66" s="331" t="s">
         <v>39</v>
       </c>
-      <c r="G66" s="325"/>
-      <c r="H66" s="325"/>
-      <c r="I66" s="326"/>
-      <c r="J66" s="324" t="s">
+      <c r="G66" s="332"/>
+      <c r="H66" s="332"/>
+      <c r="I66" s="333"/>
+      <c r="J66" s="331" t="s">
         <v>40</v>
       </c>
-      <c r="K66" s="325"/>
-      <c r="L66" s="325"/>
-      <c r="M66" s="326"/>
+      <c r="K66" s="332"/>
+      <c r="L66" s="332"/>
+      <c r="M66" s="333"/>
     </row>
     <row r="67" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B67" s="82"/>
-      <c r="D67" s="322"/>
-      <c r="E67" s="323"/>
+      <c r="D67" s="329"/>
+      <c r="E67" s="330"/>
       <c r="F67" s="83" t="s">
         <v>41</v>
       </c>
@@ -5557,8 +5644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6827,7 +6914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7752,10 +7839,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O592"/>
+  <dimension ref="A1:Q592"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A369" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E383" sqref="E383"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A431" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M466" sqref="M466:O466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7813,10 +7900,10 @@
     </row>
     <row r="5" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="82"/>
-      <c r="D5" s="322" t="s">
+      <c r="D5" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="323"/>
+      <c r="E5" s="330"/>
       <c r="F5" s="178" t="s">
         <v>125</v>
       </c>
@@ -8334,10 +8421,10 @@
     </row>
     <row r="38" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="82"/>
-      <c r="D38" s="322" t="s">
+      <c r="D38" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="323"/>
+      <c r="E38" s="330"/>
       <c r="F38" s="178" t="s">
         <v>125</v>
       </c>
@@ -8883,10 +8970,10 @@
     </row>
     <row r="72" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="82"/>
-      <c r="D72" s="322" t="s">
+      <c r="D72" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E72" s="323"/>
+      <c r="E72" s="330"/>
       <c r="F72" s="152" t="s">
         <v>126</v>
       </c>
@@ -9035,10 +9122,10 @@
     </row>
     <row r="82" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B82" s="82"/>
-      <c r="D82" s="322" t="s">
+      <c r="D82" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E82" s="323"/>
+      <c r="E82" s="330"/>
       <c r="F82" s="178" t="s">
         <v>132</v>
       </c>
@@ -9547,7 +9634,7 @@
       <c r="J112" s="150"/>
       <c r="K112" s="201"/>
     </row>
-    <row r="113" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B113" s="2"/>
       <c r="E113" s="202" t="s">
         <v>132</v>
@@ -9577,18 +9664,18 @@
         <v>0.99900000000000011</v>
       </c>
     </row>
-    <row r="114" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B115" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="116" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B116" s="82"/>
-      <c r="D116" s="322" t="s">
+      <c r="D116" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E116" s="323"/>
+      <c r="E116" s="330"/>
       <c r="F116" s="178" t="s">
         <v>132</v>
       </c>
@@ -9608,7 +9695,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="117" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B117" s="2"/>
       <c r="D117" s="87" t="s">
         <v>29</v>
@@ -9634,8 +9721,9 @@
       <c r="K117" s="146">
         <v>168835</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M117"/>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D118" s="97" t="s">
         <v>30</v>
       </c>
@@ -9660,8 +9748,9 @@
       <c r="K118" s="106">
         <v>4110</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M118"/>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D119" s="97" t="s">
         <v>95</v>
       </c>
@@ -9686,8 +9775,9 @@
       <c r="K119" s="106">
         <v>61356</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M119"/>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D120" s="97" t="s">
         <v>96</v>
       </c>
@@ -9712,8 +9802,9 @@
       <c r="K120" s="106">
         <v>4914</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M120"/>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="D121" s="97" t="s">
         <v>97</v>
@@ -9739,8 +9830,9 @@
       <c r="K121" s="106">
         <v>2287</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M121"/>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="D122" s="97" t="s">
         <v>99</v>
@@ -9766,8 +9858,9 @@
       <c r="K122" s="106">
         <v>95223</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M122"/>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="D123" s="97" t="s">
         <v>100</v>
@@ -9793,8 +9886,9 @@
       <c r="K123" s="106">
         <v>15734</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M123"/>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="D124" s="97" t="s">
         <v>101</v>
@@ -9820,8 +9914,9 @@
       <c r="K124" s="106">
         <v>3393</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M124"/>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="D125" s="97" t="s">
         <v>102</v>
@@ -9847,8 +9942,9 @@
       <c r="K125" s="106">
         <v>758</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M125"/>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="D126" s="97" t="s">
         <v>103</v>
@@ -9874,8 +9970,9 @@
       <c r="K126" s="106">
         <v>2599</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M126"/>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="D127" s="97"/>
       <c r="E127" s="186"/>
@@ -9886,7 +9983,7 @@
       <c r="J127" s="105"/>
       <c r="K127" s="106"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="D128" s="97"/>
       <c r="E128" s="186"/>
@@ -10075,7 +10172,7 @@
       <c r="J144" s="105"/>
       <c r="K144" s="106"/>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" s="3"/>
       <c r="D145" s="97"/>
       <c r="E145" s="186"/>
@@ -10086,7 +10183,7 @@
       <c r="J145" s="105"/>
       <c r="K145" s="106"/>
     </row>
-    <row r="146" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B146" s="2"/>
       <c r="D146" s="107"/>
       <c r="E146" s="189"/>
@@ -10097,7 +10194,7 @@
       <c r="J146" s="115"/>
       <c r="K146" s="116"/>
     </row>
-    <row r="147" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B147" s="2"/>
       <c r="E147" s="202" t="s">
         <v>132</v>
@@ -10127,7 +10224,7 @@
         <v>359209</v>
       </c>
     </row>
-    <row r="148" spans="1:15" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B148" s="40"/>
       <c r="D148" s="39" t="s">
         <v>50</v>
@@ -10144,7 +10241,7 @@
       <c r="N148" s="41"/>
       <c r="O148" s="41"/>
     </row>
-    <row r="149" spans="1:15" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B149" s="40"/>
       <c r="E149" s="41"/>
       <c r="F149" s="41"/>
@@ -10158,7 +10255,7 @@
       <c r="N149" s="41"/>
       <c r="O149" s="41"/>
     </row>
-    <row r="150" spans="1:15" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>137</v>
       </c>
@@ -10171,34 +10268,34 @@
       <c r="J150" s="137"/>
       <c r="K150" s="8"/>
     </row>
-    <row r="151" spans="1:15" ht="18" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" ht="18" x14ac:dyDescent="0.3">
       <c r="B151" s="9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="152" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B152" s="82"/>
-      <c r="D152" s="320" t="s">
+      <c r="D152" s="327" t="s">
         <v>56</v>
       </c>
-      <c r="E152" s="321"/>
-      <c r="F152" s="324" t="s">
+      <c r="E152" s="328"/>
+      <c r="F152" s="331" t="s">
         <v>36</v>
       </c>
-      <c r="G152" s="325"/>
-      <c r="H152" s="325"/>
-      <c r="I152" s="326"/>
-      <c r="J152" s="324" t="s">
+      <c r="G152" s="332"/>
+      <c r="H152" s="332"/>
+      <c r="I152" s="333"/>
+      <c r="J152" s="331" t="s">
         <v>40</v>
       </c>
-      <c r="K152" s="325"/>
-      <c r="L152" s="325"/>
-      <c r="M152" s="326"/>
-    </row>
-    <row r="153" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K152" s="332"/>
+      <c r="L152" s="332"/>
+      <c r="M152" s="333"/>
+    </row>
+    <row r="153" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B153" s="82"/>
-      <c r="D153" s="322"/>
-      <c r="E153" s="323"/>
+      <c r="D153" s="329"/>
+      <c r="E153" s="330"/>
       <c r="F153" s="83" t="s">
         <v>41</v>
       </c>
@@ -10220,7 +10317,7 @@
       </c>
       <c r="M153" s="86"/>
     </row>
-    <row r="154" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B154" s="2"/>
       <c r="D154" s="87" t="s">
         <v>29</v>
@@ -10248,8 +10345,20 @@
         <v>16049</v>
       </c>
       <c r="M154" s="96"/>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O154" s="326">
+        <f>+F154/SUM($F154:$H154)</f>
+        <v>0.13947368421052631</v>
+      </c>
+      <c r="P154" s="326">
+        <f t="shared" ref="P154:Q154" si="3">+G154/SUM($F154:$H154)</f>
+        <v>0.68947368421052635</v>
+      </c>
+      <c r="Q154" s="326">
+        <f t="shared" si="3"/>
+        <v>0.17105263157894737</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D155" s="97" t="s">
         <v>30</v>
       </c>
@@ -10276,8 +10385,20 @@
         <v>11966</v>
       </c>
       <c r="M155" s="106"/>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O155" s="326">
+        <f t="shared" ref="O155:O163" si="4">+F155/SUM($F155:$H155)</f>
+        <v>0.58579881656804744</v>
+      </c>
+      <c r="P155" s="326">
+        <f t="shared" ref="P155:P163" si="5">+G155/SUM($F155:$H155)</f>
+        <v>0.13017751479289941</v>
+      </c>
+      <c r="Q155" s="326">
+        <f t="shared" ref="Q155:Q163" si="6">+H155/SUM($F155:$H155)</f>
+        <v>0.28402366863905326</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D156" s="97" t="s">
         <v>95</v>
       </c>
@@ -10304,8 +10425,20 @@
         <v>41948</v>
       </c>
       <c r="M156" s="106"/>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O156" s="326">
+        <f t="shared" si="4"/>
+        <v>0.25858951175406869</v>
+      </c>
+      <c r="P156" s="326">
+        <f t="shared" si="5"/>
+        <v>0.4339963833634719</v>
+      </c>
+      <c r="Q156" s="326">
+        <f t="shared" si="6"/>
+        <v>0.30741410488245929</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D157" s="97" t="s">
         <v>96</v>
       </c>
@@ -10332,8 +10465,20 @@
         <v>77926</v>
       </c>
       <c r="M157" s="106"/>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O157" s="326">
+        <f t="shared" si="4"/>
+        <v>0.40082079343365251</v>
+      </c>
+      <c r="P157" s="326">
+        <f t="shared" si="5"/>
+        <v>0.16689466484268126</v>
+      </c>
+      <c r="Q157" s="326">
+        <f t="shared" si="6"/>
+        <v>0.4322845417236662</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" s="3"/>
       <c r="D158" s="97" t="s">
         <v>97</v>
@@ -10361,8 +10506,20 @@
         <v>39359</v>
       </c>
       <c r="M158" s="106"/>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O158" s="326">
+        <f t="shared" si="4"/>
+        <v>0.36021505376344087</v>
+      </c>
+      <c r="P158" s="326">
+        <f t="shared" si="5"/>
+        <v>0.21236559139784947</v>
+      </c>
+      <c r="Q158" s="326">
+        <f t="shared" si="6"/>
+        <v>0.42741935483870969</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" s="3"/>
       <c r="D159" s="97" t="s">
         <v>99</v>
@@ -10390,8 +10547,20 @@
         <v>16513</v>
       </c>
       <c r="M159" s="106"/>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O159" s="326">
+        <f t="shared" si="4"/>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="P159" s="326">
+        <f t="shared" si="5"/>
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="Q159" s="326">
+        <f t="shared" si="6"/>
+        <v>0.27916666666666667</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" s="3"/>
       <c r="D160" s="97" t="s">
         <v>100</v>
@@ -10419,8 +10588,20 @@
         <v>9098</v>
       </c>
       <c r="M160" s="106"/>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O160" s="326">
+        <f t="shared" si="4"/>
+        <v>0.16831683168316833</v>
+      </c>
+      <c r="P160" s="326">
+        <f t="shared" si="5"/>
+        <v>0.46534653465346532</v>
+      </c>
+      <c r="Q160" s="326">
+        <f t="shared" si="6"/>
+        <v>0.36633663366336627</v>
+      </c>
+    </row>
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" s="3"/>
       <c r="D161" s="97" t="s">
         <v>101</v>
@@ -10448,8 +10629,20 @@
         <v>22838</v>
       </c>
       <c r="M161" s="106"/>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O161" s="326">
+        <f t="shared" si="4"/>
+        <v>0.49342105263157893</v>
+      </c>
+      <c r="P161" s="326">
+        <f t="shared" si="5"/>
+        <v>0.20065789473684212</v>
+      </c>
+      <c r="Q161" s="326">
+        <f t="shared" si="6"/>
+        <v>0.30592105263157893</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" s="3"/>
       <c r="D162" s="97" t="s">
         <v>102</v>
@@ -10477,8 +10670,20 @@
         <v>1410</v>
       </c>
       <c r="M162" s="106"/>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O162" s="326">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P162" s="326">
+        <f t="shared" si="5"/>
+        <v>0.22727272727272729</v>
+      </c>
+      <c r="Q162" s="326">
+        <f t="shared" si="6"/>
+        <v>0.27272727272727276</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" s="3"/>
       <c r="D163" s="97" t="s">
         <v>103</v>
@@ -10506,8 +10711,20 @@
         <v>9711</v>
       </c>
       <c r="M163" s="106"/>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O163" s="326">
+        <f t="shared" si="4"/>
+        <v>0.58914728682170536</v>
+      </c>
+      <c r="P163" s="326">
+        <f t="shared" si="5"/>
+        <v>0.10852713178294573</v>
+      </c>
+      <c r="Q163" s="326">
+        <f t="shared" si="6"/>
+        <v>0.30232558139534882</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" s="3"/>
       <c r="D164" s="97"/>
       <c r="E164" s="186"/>
@@ -10520,7 +10737,7 @@
       <c r="L164" s="105"/>
       <c r="M164" s="106"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" s="3"/>
       <c r="D165" s="97"/>
       <c r="E165" s="186"/>
@@ -10533,7 +10750,7 @@
       <c r="L165" s="105"/>
       <c r="M165" s="106"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" s="3"/>
       <c r="D166" s="97"/>
       <c r="E166" s="186"/>
@@ -10546,7 +10763,7 @@
       <c r="L166" s="105"/>
       <c r="M166" s="106"/>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" s="3"/>
       <c r="D167" s="97"/>
       <c r="E167" s="186"/>
@@ -10559,7 +10776,7 @@
       <c r="L167" s="105"/>
       <c r="M167" s="106"/>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A168" s="3"/>
       <c r="D168" s="97"/>
       <c r="E168" s="186"/>
@@ -10572,7 +10789,7 @@
       <c r="L168" s="105"/>
       <c r="M168" s="106"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" s="3"/>
       <c r="D169" s="97"/>
       <c r="E169" s="186"/>
@@ -10585,7 +10802,7 @@
       <c r="L169" s="105"/>
       <c r="M169" s="106"/>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170" s="3"/>
       <c r="D170" s="97"/>
       <c r="E170" s="186"/>
@@ -10598,7 +10815,7 @@
       <c r="L170" s="105"/>
       <c r="M170" s="106"/>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" s="3"/>
       <c r="D171" s="97"/>
       <c r="E171" s="186"/>
@@ -10611,7 +10828,7 @@
       <c r="L171" s="105"/>
       <c r="M171" s="106"/>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" s="3"/>
       <c r="D172" s="97"/>
       <c r="E172" s="186"/>
@@ -10624,7 +10841,7 @@
       <c r="L172" s="105"/>
       <c r="M172" s="106"/>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="3"/>
       <c r="D173" s="97"/>
       <c r="E173" s="186"/>
@@ -10637,7 +10854,7 @@
       <c r="L173" s="105"/>
       <c r="M173" s="106"/>
     </row>
-    <row r="174" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="3"/>
       <c r="B174" s="2"/>
       <c r="D174" s="97"/>
@@ -10651,7 +10868,7 @@
       <c r="L174" s="105"/>
       <c r="M174" s="106"/>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="3"/>
       <c r="D175" s="97"/>
       <c r="E175" s="186"/>
@@ -10664,7 +10881,7 @@
       <c r="L175" s="105"/>
       <c r="M175" s="106"/>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" s="3"/>
       <c r="D176" s="97"/>
       <c r="E176" s="186"/>
@@ -10775,35 +10992,35 @@
         <v>132</v>
       </c>
       <c r="F184" s="235">
-        <f t="shared" ref="F184:M184" si="3">SUM(F154:F183)</f>
+        <f t="shared" ref="F184:M184" si="7">SUM(F154:F183)</f>
         <v>1.0010000000000001</v>
       </c>
       <c r="G184" s="236">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H184" s="236">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I184" s="237">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J184" s="238">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>644720</v>
       </c>
       <c r="K184" s="119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>533046</v>
       </c>
       <c r="L184" s="119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>246818</v>
       </c>
       <c r="M184" s="120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10823,27 +11040,27 @@
     </row>
     <row r="187" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B187" s="82"/>
-      <c r="D187" s="320" t="s">
+      <c r="D187" s="327" t="s">
         <v>56</v>
       </c>
-      <c r="E187" s="321"/>
-      <c r="F187" s="324" t="s">
+      <c r="E187" s="328"/>
+      <c r="F187" s="331" t="s">
         <v>39</v>
       </c>
-      <c r="G187" s="325"/>
-      <c r="H187" s="325"/>
-      <c r="I187" s="326"/>
-      <c r="J187" s="324" t="s">
+      <c r="G187" s="332"/>
+      <c r="H187" s="332"/>
+      <c r="I187" s="333"/>
+      <c r="J187" s="331" t="s">
         <v>140</v>
       </c>
-      <c r="K187" s="325"/>
-      <c r="L187" s="325"/>
-      <c r="M187" s="326"/>
+      <c r="K187" s="332"/>
+      <c r="L187" s="332"/>
+      <c r="M187" s="333"/>
     </row>
     <row r="188" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B188" s="82"/>
-      <c r="D188" s="322"/>
-      <c r="E188" s="323"/>
+      <c r="D188" s="329"/>
+      <c r="E188" s="330"/>
       <c r="F188" s="83" t="s">
         <v>41</v>
       </c>
@@ -13650,10 +13867,10 @@
     </row>
     <row r="362" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B362" s="82"/>
-      <c r="D362" s="322" t="s">
+      <c r="D362" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E362" s="323"/>
+      <c r="E362" s="330"/>
       <c r="F362" s="152" t="s">
         <v>151</v>
       </c>
@@ -13770,7 +13987,7 @@
       <c r="J368" s="3"/>
       <c r="K368" s="3"/>
     </row>
-    <row r="370" spans="1:11" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:16" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A370" s="6" t="s">
         <v>161</v>
       </c>
@@ -13783,17 +14000,17 @@
       <c r="J370" s="137"/>
       <c r="K370" s="8"/>
     </row>
-    <row r="371" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="B371" s="9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="372" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B372" s="82"/>
-      <c r="D372" s="322" t="s">
+      <c r="D372" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E372" s="323"/>
+      <c r="E372" s="330"/>
       <c r="F372" s="178" t="s">
         <v>132</v>
       </c>
@@ -13813,7 +14030,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="373" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B373" s="2"/>
       <c r="D373" s="87"/>
       <c r="E373" s="180" t="s">
@@ -13838,7 +14055,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A374" s="3"/>
       <c r="D374" s="97"/>
       <c r="E374" s="186" t="s">
@@ -13863,7 +14080,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A375" s="3"/>
       <c r="D375" s="97"/>
       <c r="E375" s="186" t="s">
@@ -13888,7 +14105,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A376" s="3"/>
       <c r="D376" s="97"/>
       <c r="E376" s="186" t="s">
@@ -13913,7 +14130,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A377" s="3"/>
       <c r="D377" s="97"/>
       <c r="E377" s="186"/>
@@ -13924,7 +14141,7 @@
       <c r="J377" s="105"/>
       <c r="K377" s="106"/>
     </row>
-    <row r="378" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B378" s="2"/>
       <c r="D378" s="107"/>
       <c r="E378" s="189"/>
@@ -13935,47 +14152,47 @@
       <c r="J378" s="115"/>
       <c r="K378" s="116"/>
     </row>
-    <row r="379" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B379" s="2"/>
       <c r="E379" s="202" t="s">
         <v>132</v>
       </c>
       <c r="F379" s="224">
-        <f t="shared" ref="F379:K379" si="4">SUM(F373:F378)</f>
+        <f t="shared" ref="F379:K379" si="8">SUM(F373:F378)</f>
         <v>25560</v>
       </c>
       <c r="G379" s="225">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5440</v>
       </c>
       <c r="H379" s="226">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4980</v>
       </c>
       <c r="I379" s="227">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5110</v>
       </c>
       <c r="J379" s="226">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5340</v>
       </c>
       <c r="K379" s="228">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4690</v>
       </c>
     </row>
-    <row r="380" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F380" s="39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A381" s="3"/>
       <c r="G381" s="79"/>
       <c r="J381" s="79"/>
     </row>
-    <row r="382" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:16" ht="18" x14ac:dyDescent="0.3">
       <c r="A382" s="3"/>
       <c r="B382" s="9" t="s">
         <v>163</v>
@@ -13983,7 +14200,7 @@
       <c r="G382" s="79"/>
       <c r="J382" s="79"/>
     </row>
-    <row r="383" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:16" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B383" s="82"/>
       <c r="E383" s="319" t="s">
         <v>56</v>
@@ -14007,7 +14224,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="384" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B384" s="2"/>
       <c r="E384" s="87" t="s">
         <v>29</v>
@@ -14030,6 +14247,8 @@
       <c r="K384" s="146">
         <v>1280</v>
       </c>
+      <c r="O384" s="324"/>
+      <c r="P384" s="325"/>
     </row>
     <row r="385" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E385" s="97" t="s">
@@ -14472,27 +14691,27 @@
         <v>132</v>
       </c>
       <c r="F414" s="224">
-        <f t="shared" ref="F414:K414" si="5">SUM(F384:F413)</f>
+        <f t="shared" ref="F414:K414" si="9">SUM(F384:F413)</f>
         <v>25560</v>
       </c>
       <c r="G414" s="225">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5440</v>
       </c>
       <c r="H414" s="226">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4980</v>
       </c>
       <c r="I414" s="227">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5110</v>
       </c>
       <c r="J414" s="226">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5340</v>
       </c>
       <c r="K414" s="228">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4690</v>
       </c>
     </row>
@@ -14514,10 +14733,10 @@
     </row>
     <row r="418" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B418" s="82"/>
-      <c r="D418" s="322" t="s">
+      <c r="D418" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E418" s="323"/>
+      <c r="E418" s="330"/>
       <c r="F418" s="138" t="s">
         <v>165</v>
       </c>
@@ -14971,10 +15190,10 @@
     </row>
     <row r="454" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B454" s="82"/>
-      <c r="D454" s="322" t="s">
+      <c r="D454" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E454" s="323"/>
+      <c r="E454" s="330"/>
       <c r="F454" s="178" t="s">
         <v>132</v>
       </c>
@@ -15135,10 +15354,10 @@
     </row>
     <row r="464" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B464" s="82"/>
-      <c r="D464" s="322" t="s">
+      <c r="D464" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E464" s="323"/>
+      <c r="E464" s="330"/>
       <c r="F464" s="178" t="s">
         <v>132</v>
       </c>
@@ -15153,7 +15372,7 @@
       </c>
       <c r="J464" s="164"/>
     </row>
-    <row r="465" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B465" s="2"/>
       <c r="D465" s="87" t="s">
         <v>29</v>
@@ -15175,7 +15394,7 @@
       </c>
       <c r="J465" s="265"/>
     </row>
-    <row r="466" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D466" s="97" t="s">
         <v>30</v>
       </c>
@@ -15196,8 +15415,20 @@
       </c>
       <c r="J466" s="266"/>
       <c r="K466" s="3"/>
-    </row>
-    <row r="467" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M466" s="339">
+        <f>+G466/$F$466</f>
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="N466" s="339">
+        <f t="shared" ref="N466:O466" si="10">+H466/$F$466</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="O466" s="339">
+        <f t="shared" si="10"/>
+        <v>0.14814814814814814</v>
+      </c>
+    </row>
+    <row r="467" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D467" s="97" t="s">
         <v>95</v>
       </c>
@@ -15219,7 +15450,7 @@
       <c r="J467" s="266"/>
       <c r="K467" s="3"/>
     </row>
-    <row r="468" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D468" s="97" t="s">
         <v>96</v>
       </c>
@@ -15241,7 +15472,7 @@
       <c r="J468" s="266"/>
       <c r="K468" s="3"/>
     </row>
-    <row r="469" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A469" s="3"/>
       <c r="D469" s="97" t="s">
         <v>97</v>
@@ -15264,7 +15495,7 @@
       <c r="J469" s="266"/>
       <c r="K469" s="3"/>
     </row>
-    <row r="470" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A470" s="3"/>
       <c r="D470" s="97" t="s">
         <v>99</v>
@@ -15287,7 +15518,7 @@
       <c r="J470" s="266"/>
       <c r="K470" s="3"/>
     </row>
-    <row r="471" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A471" s="3"/>
       <c r="D471" s="97" t="s">
         <v>100</v>
@@ -15310,7 +15541,7 @@
       <c r="J471" s="266"/>
       <c r="K471" s="3"/>
     </row>
-    <row r="472" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A472" s="3"/>
       <c r="D472" s="97" t="s">
         <v>101</v>
@@ -15333,7 +15564,7 @@
       <c r="J472" s="266"/>
       <c r="K472" s="3"/>
     </row>
-    <row r="473" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A473" s="3"/>
       <c r="D473" s="97" t="s">
         <v>102</v>
@@ -15356,7 +15587,7 @@
       <c r="J473" s="266"/>
       <c r="K473" s="3"/>
     </row>
-    <row r="474" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A474" s="3"/>
       <c r="D474" s="97" t="s">
         <v>103</v>
@@ -15379,7 +15610,7 @@
       <c r="J474" s="266"/>
       <c r="K474" s="3"/>
     </row>
-    <row r="475" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A475" s="3"/>
       <c r="D475" s="97"/>
       <c r="E475" s="186"/>
@@ -15390,7 +15621,7 @@
       <c r="J475" s="266"/>
       <c r="K475" s="3"/>
     </row>
-    <row r="476" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A476" s="3"/>
       <c r="D476" s="97"/>
       <c r="E476" s="186"/>
@@ -15401,7 +15632,7 @@
       <c r="J476" s="266"/>
       <c r="K476" s="3"/>
     </row>
-    <row r="477" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A477" s="3"/>
       <c r="D477" s="97"/>
       <c r="E477" s="186"/>
@@ -15412,7 +15643,7 @@
       <c r="J477" s="266"/>
       <c r="K477" s="3"/>
     </row>
-    <row r="478" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A478" s="3"/>
       <c r="D478" s="97"/>
       <c r="E478" s="186"/>
@@ -15423,7 +15654,7 @@
       <c r="J478" s="266"/>
       <c r="K478" s="3"/>
     </row>
-    <row r="479" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A479" s="3"/>
       <c r="D479" s="97"/>
       <c r="E479" s="186"/>
@@ -15434,7 +15665,7 @@
       <c r="J479" s="266"/>
       <c r="K479" s="3"/>
     </row>
-    <row r="480" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A480" s="3"/>
       <c r="D480" s="97"/>
       <c r="E480" s="186"/>
@@ -15647,10 +15878,10 @@
     </row>
     <row r="499" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B499" s="82"/>
-      <c r="D499" s="322" t="s">
+      <c r="D499" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E499" s="323"/>
+      <c r="E499" s="330"/>
       <c r="F499" s="152" t="s">
         <v>126</v>
       </c>
@@ -15762,10 +15993,10 @@
     </row>
     <row r="507" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B507" s="82"/>
-      <c r="D507" s="322" t="s">
+      <c r="D507" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E507" s="323"/>
+      <c r="E507" s="330"/>
       <c r="F507" s="277" t="s">
         <v>126</v>
       </c>
@@ -15871,10 +16102,10 @@
     </row>
     <row r="515" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B515" s="82"/>
-      <c r="D515" s="322" t="s">
+      <c r="D515" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E515" s="322"/>
+      <c r="E515" s="329"/>
       <c r="F515" s="281"/>
     </row>
     <row r="516" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -15963,10 +16194,10 @@
     </row>
     <row r="525" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B525" s="82"/>
-      <c r="D525" s="322" t="s">
+      <c r="D525" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E525" s="323"/>
+      <c r="E525" s="330"/>
       <c r="F525" s="152" t="s">
         <v>41</v>
       </c>
@@ -16063,10 +16294,10 @@
     </row>
     <row r="533" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B533" s="82"/>
-      <c r="D533" s="322" t="s">
+      <c r="D533" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E533" s="323"/>
+      <c r="E533" s="330"/>
       <c r="F533" s="152" t="s">
         <v>41</v>
       </c>
@@ -16155,10 +16386,10 @@
     </row>
     <row r="541" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B541" s="82"/>
-      <c r="D541" s="322" t="s">
+      <c r="D541" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E541" s="322"/>
+      <c r="E541" s="329"/>
       <c r="F541" s="281"/>
     </row>
     <row r="542" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -16248,28 +16479,28 @@
     </row>
     <row r="551" spans="1:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B551" s="9"/>
-      <c r="F551" s="329" t="s">
+      <c r="F551" s="336" t="s">
         <v>184</v>
       </c>
-      <c r="G551" s="330"/>
-      <c r="H551" s="331"/>
-      <c r="I551" s="329" t="s">
+      <c r="G551" s="337"/>
+      <c r="H551" s="338"/>
+      <c r="I551" s="336" t="s">
         <v>185</v>
       </c>
-      <c r="J551" s="330"/>
-      <c r="K551" s="331"/>
-      <c r="L551" s="329" t="s">
+      <c r="J551" s="337"/>
+      <c r="K551" s="338"/>
+      <c r="L551" s="336" t="s">
         <v>186</v>
       </c>
-      <c r="M551" s="330"/>
-      <c r="N551" s="331"/>
+      <c r="M551" s="337"/>
+      <c r="N551" s="338"/>
     </row>
     <row r="552" spans="1:14" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B552" s="82"/>
-      <c r="D552" s="322" t="s">
+      <c r="D552" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E552" s="322"/>
+      <c r="E552" s="329"/>
       <c r="F552" s="83" t="s">
         <v>5</v>
       </c>
@@ -16323,15 +16554,15 @@
         <v>0.13</v>
       </c>
       <c r="L553" s="289">
-        <f t="shared" ref="L553:N557" si="6">IF(F553=0,"",IF(F$558=0,"",F553/F$558))</f>
+        <f t="shared" ref="L553:N557" si="11">IF(F553=0,"",IF(F$558=0,"",F553/F$558))</f>
         <v>0.15017543859649124</v>
       </c>
       <c r="M553" s="155">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.14924506387921022</v>
       </c>
       <c r="N553" s="270">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.15865384615384615</v>
       </c>
     </row>
@@ -16360,15 +16591,15 @@
         <v>0.187</v>
       </c>
       <c r="L554" s="233">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.20842105263157895</v>
       </c>
       <c r="M554" s="158">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.23286875725900116</v>
       </c>
       <c r="N554" s="272">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.2796474358974359</v>
       </c>
     </row>
@@ -16397,15 +16628,15 @@
         <v>1.4E-2</v>
       </c>
       <c r="L555" s="233">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.20350877192982456</v>
       </c>
       <c r="M555" s="158">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.19221835075493612</v>
       </c>
       <c r="N555" s="272">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.12459935897435898</v>
       </c>
     </row>
@@ -16434,15 +16665,15 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="L556" s="233">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.18596491228070175</v>
       </c>
       <c r="M556" s="158">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.1759581881533101</v>
       </c>
       <c r="N556" s="272">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.13301282051282051</v>
       </c>
     </row>
@@ -16471,15 +16702,15 @@
         <v>0.161</v>
       </c>
       <c r="L557" s="234">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.2519298245614035</v>
       </c>
       <c r="M557" s="274">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.24970963995354239</v>
       </c>
       <c r="N557" s="275">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.30408653846153844</v>
       </c>
     </row>
@@ -16552,10 +16783,10 @@
     </row>
     <row r="563" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B563" s="82"/>
-      <c r="D563" s="322" t="s">
+      <c r="D563" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E563" s="323"/>
+      <c r="E563" s="330"/>
       <c r="F563" s="152" t="s">
         <v>126</v>
       </c>
@@ -16696,29 +16927,29 @@
     <row r="571" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A571" s="3"/>
       <c r="B571" s="9"/>
-      <c r="F571" s="327" t="s">
+      <c r="F571" s="334" t="s">
         <v>194</v>
       </c>
-      <c r="G571" s="328"/>
-      <c r="H571" s="327" t="s">
+      <c r="G571" s="335"/>
+      <c r="H571" s="334" t="s">
         <v>196</v>
       </c>
-      <c r="I571" s="328"/>
-      <c r="J571" s="327" t="s">
+      <c r="I571" s="335"/>
+      <c r="J571" s="334" t="s">
         <v>110</v>
       </c>
-      <c r="K571" s="328"/>
-      <c r="L571" s="327" t="s">
+      <c r="K571" s="335"/>
+      <c r="L571" s="334" t="s">
         <v>143</v>
       </c>
-      <c r="M571" s="328"/>
+      <c r="M571" s="335"/>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A572" s="3"/>
-      <c r="D572" s="322" t="s">
+      <c r="D572" s="329" t="s">
         <v>56</v>
       </c>
-      <c r="E572" s="323"/>
+      <c r="E572" s="330"/>
       <c r="F572" s="297" t="s">
         <v>197</v>
       </c>
@@ -17344,11 +17575,17 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="L551:N551"/>
+    <mergeCell ref="D515:E515"/>
+    <mergeCell ref="D525:E525"/>
+    <mergeCell ref="D533:E533"/>
+    <mergeCell ref="D541:E541"/>
+    <mergeCell ref="H571:I571"/>
+    <mergeCell ref="J571:K571"/>
+    <mergeCell ref="D563:E563"/>
+    <mergeCell ref="D507:E507"/>
+    <mergeCell ref="F551:H551"/>
+    <mergeCell ref="I551:K551"/>
     <mergeCell ref="D572:E572"/>
     <mergeCell ref="F187:I187"/>
     <mergeCell ref="J187:M187"/>
@@ -17365,17 +17602,11 @@
     <mergeCell ref="D418:E418"/>
     <mergeCell ref="L571:M571"/>
     <mergeCell ref="F571:G571"/>
-    <mergeCell ref="H571:I571"/>
-    <mergeCell ref="J571:K571"/>
-    <mergeCell ref="D563:E563"/>
-    <mergeCell ref="D507:E507"/>
-    <mergeCell ref="F551:H551"/>
-    <mergeCell ref="I551:K551"/>
-    <mergeCell ref="L551:N551"/>
-    <mergeCell ref="D515:E515"/>
-    <mergeCell ref="D525:E525"/>
-    <mergeCell ref="D533:E533"/>
-    <mergeCell ref="D541:E541"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D116:E116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17383,6 +17614,174 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C0C8F9-717F-4C78-AA24-BB82FB24CDF4}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="320" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="320" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="320" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2">
+        <v>215</v>
+      </c>
+      <c r="D2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="320" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3">
+        <v>198</v>
+      </c>
+      <c r="C3">
+        <f>+B3/B2</f>
+        <v>0.92093023255813955</v>
+      </c>
+      <c r="D3">
+        <f>+D2*C3</f>
+        <v>248.65116279069767</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="320" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4">
+        <v>63</v>
+      </c>
+      <c r="C4">
+        <f>+B4/B3</f>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="D4">
+        <f>+D3*C4</f>
+        <v>79.116279069767444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="320" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5">
+        <f>+B3-B4</f>
+        <v>135</v>
+      </c>
+      <c r="D5">
+        <f>+D3-D4</f>
+        <v>169.53488372093022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="320" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="321" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" s="321">
+        <f>+B5-B6</f>
+        <v>103</v>
+      </c>
+      <c r="D7" s="321">
+        <f>+D5-D6</f>
+        <v>104.53488372093022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="320" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="323">
+        <v>189496</v>
+      </c>
+      <c r="C9" s="323"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="320" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="323">
+        <f>+B9*B7</f>
+        <v>19518088</v>
+      </c>
+      <c r="C10" s="323"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="320"/>
+      <c r="B11" s="323"/>
+      <c r="C11" s="323"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="320"/>
+      <c r="B12" s="323"/>
+      <c r="C12" s="323"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="320" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="322">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="C13" s="323"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="320" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="323">
+        <f>+B9*B13+B9</f>
+        <v>226637.21600000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="320" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" s="323">
+        <f>+D7*B14</f>
+        <v>23691495.021395348</v>
+      </c>
+      <c r="D15" s="322">
+        <f>+B15/B10-1</f>
+        <v>0.21382253330322865</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O592"/>
   <sheetViews>
@@ -17445,10 +17844,10 @@
     </row>
     <row r="5" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="82"/>
-      <c r="D5" s="322" t="s">
+      <c r="D5" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="323"/>
+      <c r="E5" s="330"/>
       <c r="F5" s="178" t="s">
         <v>125</v>
       </c>
@@ -17804,10 +18203,10 @@
     </row>
     <row r="38" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="82"/>
-      <c r="D38" s="322" t="s">
+      <c r="D38" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="323"/>
+      <c r="E38" s="330"/>
       <c r="F38" s="178" t="s">
         <v>125</v>
       </c>
@@ -18191,10 +18590,10 @@
     </row>
     <row r="72" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="82"/>
-      <c r="D72" s="322" t="s">
+      <c r="D72" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E72" s="323"/>
+      <c r="E72" s="330"/>
       <c r="F72" s="152" t="s">
         <v>201</v>
       </c>
@@ -18305,10 +18704,10 @@
     </row>
     <row r="82" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B82" s="82"/>
-      <c r="D82" s="322" t="s">
+      <c r="D82" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E82" s="323"/>
+      <c r="E82" s="330"/>
       <c r="F82" s="178" t="s">
         <v>132</v>
       </c>
@@ -18693,10 +19092,10 @@
     </row>
     <row r="116" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B116" s="82"/>
-      <c r="D116" s="322" t="s">
+      <c r="D116" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E116" s="323"/>
+      <c r="E116" s="330"/>
       <c r="F116" s="178" t="s">
         <v>132</v>
       </c>
@@ -19124,27 +19523,27 @@
     </row>
     <row r="152" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B152" s="82"/>
-      <c r="D152" s="320" t="s">
+      <c r="D152" s="327" t="s">
         <v>74</v>
       </c>
-      <c r="E152" s="321"/>
-      <c r="F152" s="324" t="s">
+      <c r="E152" s="328"/>
+      <c r="F152" s="331" t="s">
         <v>36</v>
       </c>
-      <c r="G152" s="325"/>
-      <c r="H152" s="325"/>
-      <c r="I152" s="326"/>
-      <c r="J152" s="324" t="s">
+      <c r="G152" s="332"/>
+      <c r="H152" s="332"/>
+      <c r="I152" s="333"/>
+      <c r="J152" s="331" t="s">
         <v>40</v>
       </c>
-      <c r="K152" s="325"/>
-      <c r="L152" s="325"/>
-      <c r="M152" s="326"/>
-    </row>
-    <row r="153" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K152" s="332"/>
+      <c r="L152" s="332"/>
+      <c r="M152" s="333"/>
+    </row>
+    <row r="153" spans="1:15" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B153" s="82"/>
-      <c r="D153" s="322"/>
-      <c r="E153" s="323"/>
+      <c r="D153" s="329"/>
+      <c r="E153" s="330"/>
       <c r="F153" s="83" t="s">
         <v>41</v>
       </c>
@@ -19613,27 +20012,27 @@
     </row>
     <row r="187" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B187" s="82"/>
-      <c r="D187" s="320" t="s">
+      <c r="D187" s="327" t="s">
         <v>74</v>
       </c>
-      <c r="E187" s="321"/>
-      <c r="F187" s="324" t="s">
+      <c r="E187" s="328"/>
+      <c r="F187" s="331" t="s">
         <v>39</v>
       </c>
-      <c r="G187" s="325"/>
-      <c r="H187" s="325"/>
-      <c r="I187" s="326"/>
-      <c r="J187" s="324" t="s">
+      <c r="G187" s="332"/>
+      <c r="H187" s="332"/>
+      <c r="I187" s="333"/>
+      <c r="J187" s="331" t="s">
         <v>140</v>
       </c>
-      <c r="K187" s="325"/>
-      <c r="L187" s="325"/>
-      <c r="M187" s="326"/>
-    </row>
-    <row r="188" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K187" s="332"/>
+      <c r="L187" s="332"/>
+      <c r="M187" s="333"/>
+    </row>
+    <row r="188" spans="1:13" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B188" s="82"/>
-      <c r="D188" s="322"/>
-      <c r="E188" s="323"/>
+      <c r="D188" s="329"/>
+      <c r="E188" s="330"/>
       <c r="F188" s="83" t="s">
         <v>41</v>
       </c>
@@ -20084,10 +20483,10 @@
     </row>
     <row r="223" spans="1:13" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="82"/>
-      <c r="D223" s="322" t="s">
+      <c r="D223" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E223" s="323"/>
+      <c r="E223" s="330"/>
       <c r="F223" s="152" t="s">
         <v>75</v>
       </c>
@@ -21081,10 +21480,10 @@
     </row>
     <row r="296" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B296" s="82"/>
-      <c r="D296" s="322" t="s">
+      <c r="D296" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E296" s="323"/>
+      <c r="E296" s="330"/>
       <c r="F296" s="152" t="s">
         <v>209</v>
       </c>
@@ -21764,10 +22163,10 @@
     </row>
     <row r="362" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B362" s="82"/>
-      <c r="D362" s="322" t="s">
+      <c r="D362" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E362" s="323"/>
+      <c r="E362" s="330"/>
       <c r="F362" s="152" t="s">
         <v>209</v>
       </c>
@@ -21858,10 +22257,10 @@
     </row>
     <row r="372" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B372" s="82"/>
-      <c r="D372" s="322" t="s">
+      <c r="D372" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E372" s="323"/>
+      <c r="E372" s="330"/>
       <c r="F372" s="178" t="s">
         <v>132</v>
       </c>
@@ -21995,10 +22394,10 @@
     </row>
     <row r="383" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B383" s="82"/>
-      <c r="D383" s="322" t="s">
+      <c r="D383" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E383" s="323"/>
+      <c r="E383" s="330"/>
       <c r="F383" s="178" t="s">
         <v>132</v>
       </c>
@@ -22393,10 +22792,10 @@
     </row>
     <row r="418" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B418" s="82"/>
-      <c r="D418" s="322" t="s">
+      <c r="D418" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E418" s="323"/>
+      <c r="E418" s="330"/>
       <c r="F418" s="138" t="s">
         <v>165</v>
       </c>
@@ -22770,12 +23169,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="454" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B454" s="82"/>
-      <c r="D454" s="322" t="s">
+      <c r="D454" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E454" s="323"/>
+      <c r="E454" s="330"/>
       <c r="F454" s="178" t="s">
         <v>132</v>
       </c>
@@ -22898,10 +23297,10 @@
     </row>
     <row r="464" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B464" s="82"/>
-      <c r="D464" s="322" t="s">
+      <c r="D464" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E464" s="323"/>
+      <c r="E464" s="330"/>
       <c r="F464" s="178" t="s">
         <v>132</v>
       </c>
@@ -23292,10 +23691,10 @@
     </row>
     <row r="499" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B499" s="82"/>
-      <c r="D499" s="322" t="s">
+      <c r="D499" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E499" s="323"/>
+      <c r="E499" s="330"/>
       <c r="F499" s="152" t="s">
         <v>201</v>
       </c>
@@ -23377,10 +23776,10 @@
     </row>
     <row r="507" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B507" s="82"/>
-      <c r="D507" s="322" t="s">
+      <c r="D507" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E507" s="323"/>
+      <c r="E507" s="330"/>
       <c r="F507" s="277" t="s">
         <v>201</v>
       </c>
@@ -23456,10 +23855,10 @@
     </row>
     <row r="515" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B515" s="82"/>
-      <c r="D515" s="322" t="s">
+      <c r="D515" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E515" s="322"/>
+      <c r="E515" s="329"/>
       <c r="F515" s="281"/>
     </row>
     <row r="516" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -23538,10 +23937,10 @@
     </row>
     <row r="525" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B525" s="82"/>
-      <c r="D525" s="322" t="s">
+      <c r="D525" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E525" s="323"/>
+      <c r="E525" s="330"/>
       <c r="F525" s="152" t="s">
         <v>41</v>
       </c>
@@ -23620,10 +24019,10 @@
     </row>
     <row r="533" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B533" s="82"/>
-      <c r="D533" s="322" t="s">
+      <c r="D533" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E533" s="323"/>
+      <c r="E533" s="330"/>
       <c r="F533" s="152" t="s">
         <v>41</v>
       </c>
@@ -23694,10 +24093,10 @@
     </row>
     <row r="541" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B541" s="82"/>
-      <c r="D541" s="322" t="s">
+      <c r="D541" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E541" s="322"/>
+      <c r="E541" s="329"/>
       <c r="F541" s="281"/>
     </row>
     <row r="542" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -23777,28 +24176,28 @@
     </row>
     <row r="551" spans="1:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B551" s="9"/>
-      <c r="F551" s="329" t="s">
+      <c r="F551" s="336" t="s">
         <v>184</v>
       </c>
-      <c r="G551" s="330"/>
-      <c r="H551" s="331"/>
-      <c r="I551" s="329" t="s">
+      <c r="G551" s="337"/>
+      <c r="H551" s="338"/>
+      <c r="I551" s="336" t="s">
         <v>185</v>
       </c>
-      <c r="J551" s="330"/>
-      <c r="K551" s="331"/>
-      <c r="L551" s="329" t="s">
+      <c r="J551" s="337"/>
+      <c r="K551" s="338"/>
+      <c r="L551" s="336" t="s">
         <v>186</v>
       </c>
-      <c r="M551" s="330"/>
-      <c r="N551" s="331"/>
+      <c r="M551" s="337"/>
+      <c r="N551" s="338"/>
     </row>
     <row r="552" spans="1:14" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B552" s="82"/>
-      <c r="D552" s="322" t="s">
+      <c r="D552" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E552" s="322"/>
+      <c r="E552" s="329"/>
       <c r="F552" s="83" t="s">
         <v>5</v>
       </c>
@@ -24053,10 +24452,10 @@
     </row>
     <row r="563" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B563" s="82"/>
-      <c r="D563" s="322" t="s">
+      <c r="D563" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E563" s="323"/>
+      <c r="E563" s="330"/>
       <c r="F563" s="152" t="s">
         <v>201</v>
       </c>
@@ -24147,23 +24546,23 @@
     <row r="571" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A571" s="3"/>
       <c r="B571" s="9"/>
-      <c r="F571" s="327" t="s">
+      <c r="F571" s="334" t="s">
         <v>217</v>
       </c>
-      <c r="G571" s="328"/>
-      <c r="H571" s="327"/>
-      <c r="I571" s="328"/>
-      <c r="J571" s="327"/>
-      <c r="K571" s="328"/>
-      <c r="L571" s="327"/>
-      <c r="M571" s="328"/>
+      <c r="G571" s="335"/>
+      <c r="H571" s="334"/>
+      <c r="I571" s="335"/>
+      <c r="J571" s="334"/>
+      <c r="K571" s="335"/>
+      <c r="L571" s="334"/>
+      <c r="M571" s="335"/>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A572" s="3"/>
-      <c r="D572" s="322" t="s">
+      <c r="D572" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="E572" s="323"/>
+      <c r="E572" s="330"/>
       <c r="F572" s="297" t="s">
         <v>197</v>
       </c>
@@ -24461,6 +24860,33 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="D362:E362"/>
+    <mergeCell ref="D372:E372"/>
+    <mergeCell ref="D187:E188"/>
+    <mergeCell ref="F187:I187"/>
+    <mergeCell ref="J187:M187"/>
+    <mergeCell ref="D223:E223"/>
+    <mergeCell ref="D296:E296"/>
+    <mergeCell ref="D152:E153"/>
+    <mergeCell ref="F152:I152"/>
+    <mergeCell ref="J152:M152"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D383:E383"/>
+    <mergeCell ref="D454:E454"/>
+    <mergeCell ref="D464:E464"/>
+    <mergeCell ref="D499:E499"/>
+    <mergeCell ref="D507:E507"/>
+    <mergeCell ref="D418:E418"/>
+    <mergeCell ref="D515:E515"/>
+    <mergeCell ref="D525:E525"/>
+    <mergeCell ref="D533:E533"/>
+    <mergeCell ref="F551:H551"/>
+    <mergeCell ref="I551:K551"/>
+    <mergeCell ref="D541:E541"/>
     <mergeCell ref="D572:E572"/>
     <mergeCell ref="L551:N551"/>
     <mergeCell ref="D552:E552"/>
@@ -24469,33 +24895,6 @@
     <mergeCell ref="H571:I571"/>
     <mergeCell ref="J571:K571"/>
     <mergeCell ref="L571:M571"/>
-    <mergeCell ref="D515:E515"/>
-    <mergeCell ref="D525:E525"/>
-    <mergeCell ref="D533:E533"/>
-    <mergeCell ref="F551:H551"/>
-    <mergeCell ref="I551:K551"/>
-    <mergeCell ref="D541:E541"/>
-    <mergeCell ref="D383:E383"/>
-    <mergeCell ref="D454:E454"/>
-    <mergeCell ref="D464:E464"/>
-    <mergeCell ref="D499:E499"/>
-    <mergeCell ref="D507:E507"/>
-    <mergeCell ref="D418:E418"/>
-    <mergeCell ref="D152:E153"/>
-    <mergeCell ref="F152:I152"/>
-    <mergeCell ref="J152:M152"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D362:E362"/>
-    <mergeCell ref="D372:E372"/>
-    <mergeCell ref="D187:E188"/>
-    <mergeCell ref="F187:I187"/>
-    <mergeCell ref="J187:M187"/>
-    <mergeCell ref="D223:E223"/>
-    <mergeCell ref="D296:E296"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>